<commit_message>
JM worked on proII baseline
</commit_message>
<xml_diff>
--- a/DataExtraction1/ProIIExtractedFiles/Bulk Phase.xlsx
+++ b/DataExtraction1/ProIIExtractedFiles/Bulk Phase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\repos\datatransfer-ProII\DataExtraction1\ProIIExtractedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{15F9737B-17A1-4AEA-8D5C-C008AF19C953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C995BD4-FC34-4D10-9455-6D86F13293F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FFD167D-F6B7-4916-B172-BEB53CF408CD}"/>
   </bookViews>
@@ -1805,7 +1805,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2676,17 +2676,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8FE8C9-9311-482B-AED2-068074191707}">
   <dimension ref="A1:F524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="J187" sqref="J187"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="29.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>479</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0.34524899999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>479</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>479</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>479</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>479</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>479</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>479</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>479</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>479</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>479</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>479</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>479</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>479</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>479</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>479</v>
       </c>
@@ -2954,14 +2954,17 @@
       <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="E16">
+        <v>65.12171031954</v>
       </c>
       <c r="F16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>479</v>
       </c>
@@ -2975,7 +2978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>479</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>479</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>479</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>479</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>479</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>479</v>
       </c>
@@ -3080,7 +3083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>479</v>
       </c>
@@ -3094,7 +3097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>479</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>479</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>479</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>479</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>479</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>479</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>479</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>479</v>
       </c>
@@ -3236,7 +3239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>479</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>479</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>479</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>479</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>479</v>
       </c>
@@ -3330,7 +3333,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>479</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>479</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>479</v>
       </c>
@@ -3387,7 +3390,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>479</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>479</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>479</v>
       </c>
@@ -3432,7 +3435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>479</v>
       </c>
@@ -3449,7 +3452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>479</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>479</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>479</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>479</v>
       </c>
@@ -3514,7 +3517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>479</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>479</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>479</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>479</v>
       </c>
@@ -3582,7 +3585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>479</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>479</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>479</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>479</v>
       </c>
@@ -3659,7 +3662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>479</v>
       </c>
@@ -3676,7 +3679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>479</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>479</v>
       </c>
@@ -3713,7 +3716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>479</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>479</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>479</v>
       </c>
@@ -3764,7 +3767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>479</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>479</v>
       </c>
@@ -3801,7 +3804,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>479</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>479</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>479</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>479</v>
       </c>
@@ -3881,7 +3884,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>479</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>479</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>479</v>
       </c>
@@ -3941,7 +3944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>479</v>
       </c>
@@ -3961,7 +3964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>479</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>479</v>
       </c>
@@ -4001,7 +4004,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>479</v>
       </c>
@@ -4021,7 +4024,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>479</v>
       </c>
@@ -4041,7 +4044,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>479</v>
       </c>
@@ -4061,7 +4064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>479</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>479</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>479</v>
       </c>
@@ -4121,7 +4124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>479</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>479</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>479</v>
       </c>
@@ -4181,7 +4184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>479</v>
       </c>
@@ -4201,7 +4204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>479</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>479</v>
       </c>
@@ -4241,7 +4244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>479</v>
       </c>
@@ -4261,7 +4264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>479</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>479</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90">
         <v>479</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91">
         <v>479</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92">
         <v>479</v>
       </c>
@@ -4361,7 +4364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93">
         <v>479</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94">
         <v>479</v>
       </c>
@@ -4401,7 +4404,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95">
         <v>479</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96">
         <v>479</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97">
         <v>479</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98">
         <v>479</v>
       </c>
@@ -4481,7 +4484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99">
         <v>479</v>
       </c>
@@ -4501,7 +4504,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100">
         <v>479</v>
       </c>
@@ -4521,7 +4524,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101">
         <v>479</v>
       </c>
@@ -4541,7 +4544,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102">
         <v>479</v>
       </c>
@@ -4561,7 +4564,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103">
         <v>479</v>
       </c>
@@ -4581,7 +4584,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104">
         <v>479</v>
       </c>
@@ -4601,7 +4604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105">
         <v>479</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106">
         <v>479</v>
       </c>
@@ -4641,7 +4644,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107">
         <v>479</v>
       </c>
@@ -4658,7 +4661,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108">
         <v>479</v>
       </c>
@@ -4675,7 +4678,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109">
         <v>479</v>
       </c>
@@ -4692,7 +4695,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110">
         <v>479</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111">
         <v>479</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112">
         <v>479</v>
       </c>
@@ -4743,7 +4746,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113">
         <v>479</v>
       </c>
@@ -4760,7 +4763,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114">
         <v>479</v>
       </c>
@@ -4777,7 +4780,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115">
         <v>479</v>
       </c>
@@ -4794,7 +4797,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116">
         <v>479</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117">
         <v>479</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118">
         <v>479</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119">
         <v>479</v>
       </c>
@@ -4862,7 +4865,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120">
         <v>479</v>
       </c>
@@ -4879,7 +4882,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121">
         <v>479</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122">
         <v>479</v>
       </c>
@@ -4913,7 +4916,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123">
         <v>479</v>
       </c>
@@ -4930,7 +4933,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124">
         <v>479</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125">
         <v>479</v>
       </c>
@@ -4964,7 +4967,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126">
         <v>479</v>
       </c>
@@ -4981,7 +4984,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127">
         <v>479</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128">
         <v>479</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129">
         <v>479</v>
       </c>
@@ -5032,7 +5035,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="A130">
         <v>479</v>
       </c>
@@ -5049,7 +5052,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="A131">
         <v>479</v>
       </c>
@@ -5066,7 +5069,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="A132">
         <v>479</v>
       </c>
@@ -5083,7 +5086,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="A133">
         <v>479</v>
       </c>
@@ -5100,7 +5103,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134">
         <v>479</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="A135">
         <v>479</v>
       </c>
@@ -5137,7 +5140,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6">
       <c r="A136">
         <v>479</v>
       </c>
@@ -5157,7 +5160,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6">
       <c r="A137">
         <v>479</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6">
       <c r="A138">
         <v>479</v>
       </c>
@@ -5197,7 +5200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6">
       <c r="A139">
         <v>479</v>
       </c>
@@ -5217,7 +5220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6">
       <c r="A140">
         <v>479</v>
       </c>
@@ -5237,7 +5240,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6">
       <c r="A141">
         <v>479</v>
       </c>
@@ -5257,7 +5260,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6">
       <c r="A142">
         <v>479</v>
       </c>
@@ -5277,7 +5280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6">
       <c r="A143">
         <v>479</v>
       </c>
@@ -5297,7 +5300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6">
       <c r="A144">
         <v>479</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="A145">
         <v>479</v>
       </c>
@@ -5337,7 +5340,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="A146">
         <v>479</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="A147">
         <v>479</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="A148">
         <v>479</v>
       </c>
@@ -5397,7 +5400,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149">
         <v>479</v>
       </c>
@@ -5417,7 +5420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="A150">
         <v>479</v>
       </c>
@@ -5437,7 +5440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="A151">
         <v>479</v>
       </c>
@@ -5457,7 +5460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="A152">
         <v>479</v>
       </c>
@@ -5477,7 +5480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="A153">
         <v>479</v>
       </c>
@@ -5497,7 +5500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="A154">
         <v>479</v>
       </c>
@@ -5517,7 +5520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="A155">
         <v>479</v>
       </c>
@@ -5537,7 +5540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="A156">
         <v>479</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="A157">
         <v>479</v>
       </c>
@@ -5577,7 +5580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="A158">
         <v>479</v>
       </c>
@@ -5597,7 +5600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="A159">
         <v>479</v>
       </c>
@@ -5617,7 +5620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="A160">
         <v>479</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6">
       <c r="A161">
         <v>479</v>
       </c>
@@ -5657,7 +5660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6">
       <c r="A162">
         <v>479</v>
       </c>
@@ -5677,7 +5680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6">
       <c r="A163">
         <v>479</v>
       </c>
@@ -5697,7 +5700,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6">
       <c r="A164">
         <v>479</v>
       </c>
@@ -5717,7 +5720,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6">
       <c r="A165">
         <v>479</v>
       </c>
@@ -5737,7 +5740,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6">
       <c r="A166">
         <v>479</v>
       </c>
@@ -5757,7 +5760,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6">
       <c r="A167">
         <v>479</v>
       </c>
@@ -5777,7 +5780,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6">
       <c r="A168">
         <v>479</v>
       </c>
@@ -5797,7 +5800,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6">
       <c r="A169">
         <v>479</v>
       </c>
@@ -5817,7 +5820,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6">
       <c r="A170">
         <v>479</v>
       </c>
@@ -5837,7 +5840,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6">
       <c r="A171">
         <v>479</v>
       </c>
@@ -5857,7 +5860,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6">
       <c r="A172">
         <v>479</v>
       </c>
@@ -5877,7 +5880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6">
       <c r="A173">
         <v>479</v>
       </c>
@@ -5897,7 +5900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6">
       <c r="A174">
         <v>479</v>
       </c>
@@ -5917,7 +5920,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6">
       <c r="A175">
         <v>479</v>
       </c>
@@ -5937,7 +5940,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6">
       <c r="A176">
         <v>479</v>
       </c>
@@ -5957,7 +5960,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6">
       <c r="A177">
         <v>479</v>
       </c>
@@ -5974,7 +5977,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6">
       <c r="A178">
         <v>479</v>
       </c>
@@ -5991,7 +5994,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6">
       <c r="A179">
         <v>479</v>
       </c>
@@ -6008,7 +6011,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6">
       <c r="A180">
         <v>479</v>
       </c>
@@ -6025,7 +6028,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6">
       <c r="A181">
         <v>479</v>
       </c>
@@ -6042,7 +6045,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6">
       <c r="A182">
         <v>479</v>
       </c>
@@ -6059,7 +6062,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6">
       <c r="A183">
         <v>479</v>
       </c>
@@ -6076,7 +6079,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6">
       <c r="A184">
         <v>479</v>
       </c>
@@ -6093,7 +6096,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6">
       <c r="A185">
         <v>479</v>
       </c>
@@ -6110,7 +6113,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6">
       <c r="A186">
         <v>479</v>
       </c>
@@ -6127,7 +6130,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6">
       <c r="A187">
         <v>479</v>
       </c>
@@ -6144,7 +6147,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6">
       <c r="A188">
         <v>479</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6">
       <c r="A189">
         <v>479</v>
       </c>
@@ -6178,7 +6181,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6">
       <c r="A190">
         <v>479</v>
       </c>
@@ -6195,7 +6198,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6">
       <c r="A191">
         <v>479</v>
       </c>
@@ -6215,7 +6218,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192">
         <v>479</v>
       </c>
@@ -6235,7 +6238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6">
       <c r="A193">
         <v>479</v>
       </c>
@@ -6255,7 +6258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6">
       <c r="A194">
         <v>479</v>
       </c>
@@ -6275,7 +6278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6">
       <c r="A195">
         <v>479</v>
       </c>
@@ -6295,7 +6298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6">
       <c r="A196">
         <v>479</v>
       </c>
@@ -6315,7 +6318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6">
       <c r="A197">
         <v>479</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6">
       <c r="A198">
         <v>479</v>
       </c>
@@ -6355,7 +6358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6">
       <c r="A199">
         <v>479</v>
       </c>
@@ -6375,7 +6378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6">
       <c r="A200">
         <v>479</v>
       </c>
@@ -6395,7 +6398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6">
       <c r="A201">
         <v>479</v>
       </c>
@@ -6415,7 +6418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6">
       <c r="A202">
         <v>479</v>
       </c>
@@ -6435,7 +6438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6">
       <c r="A203">
         <v>479</v>
       </c>
@@ -6455,7 +6458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6">
       <c r="A204">
         <v>479</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6">
       <c r="A205">
         <v>479</v>
       </c>
@@ -6495,7 +6498,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6">
       <c r="A206">
         <v>479</v>
       </c>
@@ -6515,7 +6518,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6">
       <c r="A207">
         <v>479</v>
       </c>
@@ -6535,7 +6538,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6">
       <c r="A208">
         <v>479</v>
       </c>
@@ -6555,7 +6558,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6">
       <c r="A209">
         <v>479</v>
       </c>
@@ -6575,7 +6578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6">
       <c r="A210">
         <v>479</v>
       </c>
@@ -6595,7 +6598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6">
       <c r="A211">
         <v>479</v>
       </c>
@@ -6615,7 +6618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6">
       <c r="A212">
         <v>479</v>
       </c>
@@ -6635,7 +6638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6">
       <c r="A213">
         <v>479</v>
       </c>
@@ -6655,7 +6658,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6">
       <c r="A214">
         <v>479</v>
       </c>
@@ -6675,7 +6678,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6">
       <c r="A215">
         <v>479</v>
       </c>
@@ -6695,7 +6698,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6">
       <c r="A216">
         <v>479</v>
       </c>
@@ -6715,7 +6718,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6">
       <c r="A217">
         <v>479</v>
       </c>
@@ -6735,7 +6738,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6">
       <c r="A218">
         <v>479</v>
       </c>
@@ -6755,7 +6758,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6">
       <c r="A219">
         <v>479</v>
       </c>
@@ -6772,7 +6775,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6">
       <c r="A220">
         <v>479</v>
       </c>
@@ -6789,7 +6792,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6">
       <c r="A221">
         <v>479</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6">
       <c r="A222">
         <v>479</v>
       </c>
@@ -6823,7 +6826,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6">
       <c r="A223">
         <v>479</v>
       </c>
@@ -6840,7 +6843,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6">
       <c r="A224">
         <v>479</v>
       </c>
@@ -6857,7 +6860,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6">
       <c r="A225">
         <v>479</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6">
       <c r="A226">
         <v>479</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6">
       <c r="A227">
         <v>479</v>
       </c>
@@ -6908,7 +6911,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6">
       <c r="A228">
         <v>479</v>
       </c>
@@ -6925,7 +6928,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6">
       <c r="A229">
         <v>479</v>
       </c>
@@ -6942,7 +6945,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6">
       <c r="A230">
         <v>479</v>
       </c>
@@ -6959,7 +6962,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6">
       <c r="A231">
         <v>479</v>
       </c>
@@ -6976,7 +6979,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6">
       <c r="A232">
         <v>479</v>
       </c>
@@ -6993,7 +6996,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6">
       <c r="A233">
         <v>479</v>
       </c>
@@ -7007,7 +7010,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6">
       <c r="A234">
         <v>479</v>
       </c>
@@ -7021,7 +7024,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6">
       <c r="A235">
         <v>479</v>
       </c>
@@ -7035,7 +7038,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6">
       <c r="A236">
         <v>479</v>
       </c>
@@ -7049,7 +7052,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6">
       <c r="A237">
         <v>479</v>
       </c>
@@ -7063,7 +7066,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6">
       <c r="A238">
         <v>479</v>
       </c>
@@ -7077,7 +7080,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6">
       <c r="A239">
         <v>479</v>
       </c>
@@ -7091,7 +7094,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6">
       <c r="A240">
         <v>479</v>
       </c>
@@ -7108,7 +7111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6">
       <c r="A241">
         <v>479</v>
       </c>
@@ -7125,7 +7128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6">
       <c r="A242">
         <v>479</v>
       </c>
@@ -7142,7 +7145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6">
       <c r="A243">
         <v>479</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6">
       <c r="A244">
         <v>479</v>
       </c>
@@ -7170,7 +7173,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6">
       <c r="A245">
         <v>479</v>
       </c>
@@ -7184,7 +7187,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6">
       <c r="A246">
         <v>479</v>
       </c>
@@ -7198,7 +7201,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6">
       <c r="A247">
         <v>479</v>
       </c>
@@ -7215,7 +7218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6">
       <c r="A248">
         <v>479</v>
       </c>
@@ -7229,7 +7232,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6">
       <c r="A249">
         <v>479</v>
       </c>
@@ -7243,7 +7246,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6">
       <c r="A250">
         <v>479</v>
       </c>
@@ -7257,7 +7260,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6">
       <c r="A251">
         <v>479</v>
       </c>
@@ -7271,7 +7274,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6">
       <c r="A252">
         <v>479</v>
       </c>
@@ -7285,7 +7288,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6">
       <c r="A253">
         <v>479</v>
       </c>
@@ -7299,7 +7302,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6">
       <c r="A254">
         <v>479</v>
       </c>
@@ -7313,7 +7316,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6">
       <c r="A255">
         <v>479</v>
       </c>
@@ -7330,7 +7333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6">
       <c r="A256">
         <v>479</v>
       </c>
@@ -7347,7 +7350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6">
       <c r="A257">
         <v>479</v>
       </c>
@@ -7364,7 +7367,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6">
       <c r="A258">
         <v>479</v>
       </c>
@@ -7381,7 +7384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6">
       <c r="A259">
         <v>479</v>
       </c>
@@ -7398,7 +7401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6">
       <c r="A260">
         <v>479</v>
       </c>
@@ -7415,7 +7418,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6">
       <c r="A261">
         <v>479</v>
       </c>
@@ -7429,7 +7432,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6">
       <c r="A262">
         <v>479</v>
       </c>
@@ -7446,7 +7449,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6">
       <c r="A263">
         <v>479</v>
       </c>
@@ -7460,7 +7463,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6">
       <c r="A264">
         <v>479</v>
       </c>
@@ -7477,7 +7480,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6">
       <c r="A265">
         <v>479</v>
       </c>
@@ -7494,7 +7497,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6">
       <c r="A266">
         <v>479</v>
       </c>
@@ -7508,7 +7511,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6">
       <c r="A267">
         <v>479</v>
       </c>
@@ -7522,7 +7525,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6">
       <c r="A268">
         <v>479</v>
       </c>
@@ -7536,7 +7539,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6">
       <c r="A269">
         <v>479</v>
       </c>
@@ -7553,7 +7556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6">
       <c r="A270">
         <v>479</v>
       </c>
@@ -7570,7 +7573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6">
       <c r="A271">
         <v>479</v>
       </c>
@@ -7587,7 +7590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6">
       <c r="A272">
         <v>479</v>
       </c>
@@ -7604,7 +7607,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6">
       <c r="A273">
         <v>479</v>
       </c>
@@ -7621,7 +7624,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6">
       <c r="A274">
         <v>479</v>
       </c>
@@ -7638,7 +7641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6">
       <c r="A275">
         <v>479</v>
       </c>
@@ -7655,7 +7658,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6">
       <c r="A276">
         <v>479</v>
       </c>
@@ -7672,7 +7675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6">
       <c r="A277">
         <v>479</v>
       </c>
@@ -7689,7 +7692,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6">
       <c r="A278">
         <v>479</v>
       </c>
@@ -7703,7 +7706,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6">
       <c r="A279">
         <v>479</v>
       </c>
@@ -7720,7 +7723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6">
       <c r="A280">
         <v>479</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6">
       <c r="A281">
         <v>479</v>
       </c>
@@ -7754,7 +7757,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6">
       <c r="A282">
         <v>479</v>
       </c>
@@ -7771,7 +7774,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6">
       <c r="A283">
         <v>479</v>
       </c>
@@ -7785,7 +7788,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6">
       <c r="A284">
         <v>479</v>
       </c>
@@ -7799,7 +7802,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6">
       <c r="A285">
         <v>479</v>
       </c>
@@ -7813,7 +7816,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6">
       <c r="A286">
         <v>479</v>
       </c>
@@ -7827,7 +7830,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6">
       <c r="A287">
         <v>479</v>
       </c>
@@ -7844,7 +7847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6">
       <c r="A288">
         <v>479</v>
       </c>
@@ -7861,7 +7864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6">
       <c r="A289">
         <v>479</v>
       </c>
@@ -7878,7 +7881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6">
       <c r="A290">
         <v>479</v>
       </c>
@@ -7895,7 +7898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6">
       <c r="A291">
         <v>479</v>
       </c>
@@ -7912,7 +7915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6">
       <c r="A292">
         <v>479</v>
       </c>
@@ -7929,7 +7932,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6">
       <c r="A293">
         <v>479</v>
       </c>
@@ -7946,7 +7949,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6">
       <c r="A294">
         <v>479</v>
       </c>
@@ -7963,7 +7966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6">
       <c r="A295">
         <v>479</v>
       </c>
@@ -7980,7 +7983,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6">
       <c r="A296">
         <v>479</v>
       </c>
@@ -7997,7 +8000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6">
       <c r="A297">
         <v>479</v>
       </c>
@@ -8014,7 +8017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6">
       <c r="A298">
         <v>479</v>
       </c>
@@ -8031,7 +8034,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6">
       <c r="A299">
         <v>479</v>
       </c>
@@ -8048,7 +8051,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6">
       <c r="A300">
         <v>479</v>
       </c>
@@ -8065,7 +8068,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6">
       <c r="A301">
         <v>479</v>
       </c>
@@ -8082,7 +8085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6">
       <c r="A302">
         <v>479</v>
       </c>
@@ -8099,7 +8102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6">
       <c r="A303">
         <v>479</v>
       </c>
@@ -8113,7 +8116,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6">
       <c r="A304">
         <v>479</v>
       </c>
@@ -8127,7 +8130,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6">
       <c r="A305">
         <v>479</v>
       </c>
@@ -8141,7 +8144,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6">
       <c r="A306">
         <v>479</v>
       </c>
@@ -8155,7 +8158,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6">
       <c r="A307">
         <v>479</v>
       </c>
@@ -8172,7 +8175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6">
       <c r="A308">
         <v>479</v>
       </c>
@@ -8189,7 +8192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6">
       <c r="A309">
         <v>479</v>
       </c>
@@ -8206,7 +8209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6">
       <c r="A310">
         <v>479</v>
       </c>
@@ -8220,7 +8223,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6">
       <c r="A311">
         <v>479</v>
       </c>
@@ -8234,7 +8237,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6">
       <c r="A312">
         <v>479</v>
       </c>
@@ -8248,7 +8251,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6">
       <c r="A313">
         <v>479</v>
       </c>
@@ -8262,7 +8265,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6">
       <c r="A314">
         <v>479</v>
       </c>
@@ -8279,7 +8282,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6">
       <c r="A315">
         <v>479</v>
       </c>
@@ -8293,7 +8296,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6">
       <c r="A316">
         <v>479</v>
       </c>
@@ -8307,7 +8310,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6">
       <c r="A317">
         <v>479</v>
       </c>
@@ -8321,7 +8324,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6">
       <c r="A318">
         <v>479</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6">
       <c r="A319">
         <v>479</v>
       </c>
@@ -8349,7 +8352,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6">
       <c r="A320">
         <v>479</v>
       </c>
@@ -8363,7 +8366,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6">
       <c r="A321">
         <v>479</v>
       </c>
@@ -8377,7 +8380,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6">
       <c r="A322">
         <v>479</v>
       </c>
@@ -8394,7 +8397,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6">
       <c r="A323">
         <v>479</v>
       </c>
@@ -8411,7 +8414,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6">
       <c r="A324">
         <v>479</v>
       </c>
@@ -8428,7 +8431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6">
       <c r="A325">
         <v>479</v>
       </c>
@@ -8445,7 +8448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6">
       <c r="A326">
         <v>479</v>
       </c>
@@ -8462,7 +8465,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6">
       <c r="A327">
         <v>479</v>
       </c>
@@ -8476,7 +8479,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6">
       <c r="A328">
         <v>479</v>
       </c>
@@ -8493,7 +8496,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6">
       <c r="A329">
         <v>479</v>
       </c>
@@ -8507,7 +8510,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6">
       <c r="A330">
         <v>479</v>
       </c>
@@ -8521,7 +8524,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6">
       <c r="A331">
         <v>479</v>
       </c>
@@ -8535,7 +8538,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6">
       <c r="A332">
         <v>479</v>
       </c>
@@ -8552,7 +8555,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6">
       <c r="A333">
         <v>479</v>
       </c>
@@ -8569,7 +8572,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6">
       <c r="A334">
         <v>479</v>
       </c>
@@ -8583,7 +8586,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6">
       <c r="A335">
         <v>479</v>
       </c>
@@ -8597,7 +8600,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6">
       <c r="A336">
         <v>479</v>
       </c>
@@ -8611,7 +8614,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6">
       <c r="A337">
         <v>479</v>
       </c>
@@ -8625,7 +8628,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6">
       <c r="A338">
         <v>479</v>
       </c>
@@ -8642,7 +8645,7 @@
         <v>0.34524899999999997</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6">
       <c r="A339">
         <v>479</v>
       </c>
@@ -8656,7 +8659,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6">
       <c r="A340">
         <v>479</v>
       </c>
@@ -8670,7 +8673,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6">
       <c r="A341">
         <v>479</v>
       </c>
@@ -8690,7 +8693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6">
       <c r="A342">
         <v>479</v>
       </c>
@@ -8710,7 +8713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6">
       <c r="A343">
         <v>479</v>
       </c>
@@ -8730,7 +8733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6">
       <c r="A344">
         <v>479</v>
       </c>
@@ -8747,7 +8750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6">
       <c r="A345">
         <v>479</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6">
       <c r="A346">
         <v>479</v>
       </c>
@@ -8775,7 +8778,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6">
       <c r="A347">
         <v>479</v>
       </c>
@@ -8792,7 +8795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6">
       <c r="A348">
         <v>479</v>
       </c>
@@ -8806,7 +8809,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6">
       <c r="A349">
         <v>479</v>
       </c>
@@ -8826,7 +8829,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6">
       <c r="A350">
         <v>479</v>
       </c>
@@ -8846,7 +8849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6">
       <c r="A351">
         <v>479</v>
       </c>
@@ -8863,7 +8866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6">
       <c r="A352">
         <v>479</v>
       </c>
@@ -8883,7 +8886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6">
       <c r="A353">
         <v>479</v>
       </c>
@@ -8900,7 +8903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6">
       <c r="A354">
         <v>479</v>
       </c>
@@ -8914,7 +8917,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6">
       <c r="A355">
         <v>479</v>
       </c>
@@ -8931,7 +8934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6">
       <c r="A356">
         <v>479</v>
       </c>
@@ -8951,7 +8954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6">
       <c r="A357">
         <v>479</v>
       </c>
@@ -8971,7 +8974,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6">
       <c r="A358">
         <v>479</v>
       </c>
@@ -8991,7 +8994,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6">
       <c r="A359">
         <v>479</v>
       </c>
@@ -9008,7 +9011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6">
       <c r="A360">
         <v>479</v>
       </c>
@@ -9028,7 +9031,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6">
       <c r="A361">
         <v>479</v>
       </c>
@@ -9042,7 +9045,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6">
       <c r="A362">
         <v>479</v>
       </c>
@@ -9062,7 +9065,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6">
       <c r="A363">
         <v>479</v>
       </c>
@@ -9079,7 +9082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6">
       <c r="A364">
         <v>479</v>
       </c>
@@ -9093,7 +9096,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6">
       <c r="A365">
         <v>479</v>
       </c>
@@ -9110,7 +9113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6">
       <c r="A366">
         <v>479</v>
       </c>
@@ -9124,7 +9127,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6">
       <c r="A367">
         <v>479</v>
       </c>
@@ -9144,7 +9147,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6">
       <c r="A368">
         <v>479</v>
       </c>
@@ -9161,7 +9164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6">
       <c r="A369">
         <v>479</v>
       </c>
@@ -9181,7 +9184,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6">
       <c r="A370">
         <v>479</v>
       </c>
@@ -9201,7 +9204,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6">
       <c r="A371">
         <v>479</v>
       </c>
@@ -9218,7 +9221,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6">
       <c r="A372">
         <v>479</v>
       </c>
@@ -9238,7 +9241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6">
       <c r="A373">
         <v>479</v>
       </c>
@@ -9252,7 +9255,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6">
       <c r="A374">
         <v>479</v>
       </c>
@@ -9266,7 +9269,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6">
       <c r="A375">
         <v>479</v>
       </c>
@@ -9280,7 +9283,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6">
       <c r="A376">
         <v>479</v>
       </c>
@@ -9297,7 +9300,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6">
       <c r="A377">
         <v>479</v>
       </c>
@@ -9314,7 +9317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6">
       <c r="A378">
         <v>479</v>
       </c>
@@ -9331,7 +9334,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6">
       <c r="A379">
         <v>479</v>
       </c>
@@ -9345,7 +9348,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6">
       <c r="A380">
         <v>479</v>
       </c>
@@ -9359,7 +9362,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6">
       <c r="A381">
         <v>479</v>
       </c>
@@ -9373,7 +9376,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6">
       <c r="A382">
         <v>479</v>
       </c>
@@ -9390,7 +9393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6">
       <c r="A383">
         <v>479</v>
       </c>
@@ -9404,7 +9407,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6">
       <c r="A384">
         <v>479</v>
       </c>
@@ -9421,7 +9424,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6">
       <c r="A385">
         <v>479</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6">
       <c r="A386">
         <v>479</v>
       </c>
@@ -9455,7 +9458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6">
       <c r="A387">
         <v>479</v>
       </c>
@@ -9472,7 +9475,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6">
       <c r="A388">
         <v>479</v>
       </c>
@@ -9489,7 +9492,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6">
       <c r="A389">
         <v>479</v>
       </c>
@@ -9503,7 +9506,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6">
       <c r="A390">
         <v>479</v>
       </c>
@@ -9520,7 +9523,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6">
       <c r="A391">
         <v>479</v>
       </c>
@@ -9537,7 +9540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6">
       <c r="A392">
         <v>479</v>
       </c>
@@ -9554,7 +9557,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6">
       <c r="A393">
         <v>479</v>
       </c>
@@ -9571,7 +9574,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6">
       <c r="A394">
         <v>479</v>
       </c>
@@ -9585,7 +9588,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6">
       <c r="A395">
         <v>479</v>
       </c>
@@ -9602,7 +9605,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6">
       <c r="A396">
         <v>479</v>
       </c>
@@ -9616,7 +9619,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6">
       <c r="A397">
         <v>479</v>
       </c>
@@ -9633,7 +9636,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6">
       <c r="A398">
         <v>479</v>
       </c>
@@ -9650,7 +9653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6">
       <c r="A399">
         <v>479</v>
       </c>
@@ -9664,7 +9667,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6">
       <c r="A400">
         <v>479</v>
       </c>
@@ -9681,7 +9684,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6">
       <c r="A401">
         <v>479</v>
       </c>
@@ -9695,7 +9698,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6">
       <c r="A402">
         <v>479</v>
       </c>
@@ -9712,7 +9715,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6">
       <c r="A403">
         <v>479</v>
       </c>
@@ -9726,7 +9729,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6">
       <c r="A404">
         <v>479</v>
       </c>
@@ -9743,7 +9746,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6">
       <c r="A405">
         <v>479</v>
       </c>
@@ -9760,7 +9763,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6">
       <c r="A406">
         <v>479</v>
       </c>
@@ -9777,7 +9780,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6">
       <c r="A407">
         <v>479</v>
       </c>
@@ -9794,7 +9797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6">
       <c r="A408">
         <v>479</v>
       </c>
@@ -9811,7 +9814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6">
       <c r="A409">
         <v>479</v>
       </c>
@@ -9825,7 +9828,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6">
       <c r="A410">
         <v>479</v>
       </c>
@@ -9842,7 +9845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6">
       <c r="A411">
         <v>479</v>
       </c>
@@ -9856,7 +9859,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6">
       <c r="A412">
         <v>479</v>
       </c>
@@ -9870,7 +9873,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6">
       <c r="A413">
         <v>479</v>
       </c>
@@ -9884,7 +9887,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6">
       <c r="A414">
         <v>479</v>
       </c>
@@ -9898,7 +9901,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6">
       <c r="A415">
         <v>479</v>
       </c>
@@ -9912,7 +9915,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6">
       <c r="A416">
         <v>479</v>
       </c>
@@ -9929,7 +9932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6">
       <c r="A417">
         <v>479</v>
       </c>
@@ -9943,7 +9946,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6">
       <c r="A418">
         <v>479</v>
       </c>
@@ -9957,7 +9960,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6">
       <c r="A419">
         <v>479</v>
       </c>
@@ -9974,7 +9977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6">
       <c r="A420">
         <v>479</v>
       </c>
@@ -9988,7 +9991,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6">
       <c r="A421">
         <v>479</v>
       </c>
@@ -10002,7 +10005,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6">
       <c r="A422">
         <v>479</v>
       </c>
@@ -10019,7 +10022,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6">
       <c r="A423">
         <v>479</v>
       </c>
@@ -10036,7 +10039,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6">
       <c r="A424">
         <v>479</v>
       </c>
@@ -10053,7 +10056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6">
       <c r="A425">
         <v>479</v>
       </c>
@@ -10067,7 +10070,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6">
       <c r="A426">
         <v>479</v>
       </c>
@@ -10081,7 +10084,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6">
       <c r="A427">
         <v>479</v>
       </c>
@@ -10095,7 +10098,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6">
       <c r="A428">
         <v>479</v>
       </c>
@@ -10109,7 +10112,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6">
       <c r="A429">
         <v>479</v>
       </c>
@@ -10126,7 +10129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6">
       <c r="A430">
         <v>479</v>
       </c>
@@ -10143,7 +10146,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6">
       <c r="A431">
         <v>479</v>
       </c>
@@ -10160,7 +10163,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6">
       <c r="A432">
         <v>479</v>
       </c>
@@ -10177,7 +10180,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6">
       <c r="A433">
         <v>479</v>
       </c>
@@ -10191,7 +10194,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6">
       <c r="A434">
         <v>479</v>
       </c>
@@ -10205,7 +10208,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6">
       <c r="A435">
         <v>479</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6">
       <c r="A436">
         <v>479</v>
       </c>
@@ -10233,7 +10236,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6">
       <c r="A437">
         <v>479</v>
       </c>
@@ -10247,7 +10250,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6">
       <c r="A438">
         <v>479</v>
       </c>
@@ -10264,7 +10267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6">
       <c r="A439">
         <v>479</v>
       </c>
@@ -10278,7 +10281,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6">
       <c r="A440">
         <v>479</v>
       </c>
@@ -10295,7 +10298,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6">
       <c r="A441">
         <v>479</v>
       </c>
@@ -10312,7 +10315,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6">
       <c r="A442">
         <v>479</v>
       </c>
@@ -10329,7 +10332,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6">
       <c r="A443">
         <v>479</v>
       </c>
@@ -10343,7 +10346,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6">
       <c r="A444">
         <v>479</v>
       </c>
@@ -10357,7 +10360,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6">
       <c r="A445">
         <v>479</v>
       </c>
@@ -10371,7 +10374,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6">
       <c r="A446">
         <v>479</v>
       </c>
@@ -10385,7 +10388,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6">
       <c r="A447">
         <v>479</v>
       </c>
@@ -10399,7 +10402,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6">
       <c r="A448">
         <v>479</v>
       </c>
@@ -10413,7 +10416,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6">
       <c r="A449">
         <v>479</v>
       </c>
@@ -10427,7 +10430,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6">
       <c r="A450">
         <v>479</v>
       </c>
@@ -10444,7 +10447,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6">
       <c r="A451">
         <v>479</v>
       </c>
@@ -10458,7 +10461,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6">
       <c r="A452">
         <v>479</v>
       </c>
@@ -10472,7 +10475,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6">
       <c r="A453">
         <v>479</v>
       </c>
@@ -10486,7 +10489,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6">
       <c r="A454">
         <v>479</v>
       </c>
@@ -10500,7 +10503,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6">
       <c r="A455">
         <v>479</v>
       </c>
@@ -10514,7 +10517,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6">
       <c r="A456">
         <v>479</v>
       </c>
@@ -10528,7 +10531,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6">
       <c r="A457">
         <v>479</v>
       </c>
@@ -10542,7 +10545,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6">
       <c r="A458">
         <v>479</v>
       </c>
@@ -10559,7 +10562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6">
       <c r="A459">
         <v>479</v>
       </c>
@@ -10576,7 +10579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6">
       <c r="A460">
         <v>479</v>
       </c>
@@ -10593,7 +10596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6">
       <c r="A461">
         <v>479</v>
       </c>
@@ -10610,7 +10613,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6">
       <c r="A462">
         <v>479</v>
       </c>
@@ -10627,7 +10630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6">
       <c r="A463">
         <v>479</v>
       </c>
@@ -10644,7 +10647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6">
       <c r="A464">
         <v>479</v>
       </c>
@@ -10658,7 +10661,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6">
       <c r="A465">
         <v>479</v>
       </c>
@@ -10675,7 +10678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6">
       <c r="A466">
         <v>479</v>
       </c>
@@ -10692,7 +10695,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6">
       <c r="A467">
         <v>479</v>
       </c>
@@ -10709,7 +10712,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6">
       <c r="A468">
         <v>479</v>
       </c>
@@ -10726,7 +10729,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6">
       <c r="A469">
         <v>479</v>
       </c>
@@ -10743,7 +10746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6">
       <c r="A470">
         <v>479</v>
       </c>
@@ -10760,7 +10763,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:6">
       <c r="A471">
         <v>479</v>
       </c>
@@ -10774,7 +10777,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:6">
       <c r="A472">
         <v>479</v>
       </c>
@@ -10791,7 +10794,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6">
       <c r="A473">
         <v>479</v>
       </c>
@@ -10808,7 +10811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:6">
       <c r="A474">
         <v>479</v>
       </c>
@@ -10825,7 +10828,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:6">
       <c r="A475">
         <v>479</v>
       </c>
@@ -10842,7 +10845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:6">
       <c r="A476">
         <v>479</v>
       </c>
@@ -10859,7 +10862,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:6">
       <c r="A477">
         <v>479</v>
       </c>
@@ -10876,7 +10879,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:6">
       <c r="A478">
         <v>479</v>
       </c>
@@ -10890,7 +10893,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6">
       <c r="A479">
         <v>479</v>
       </c>
@@ -10907,7 +10910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6">
       <c r="A480">
         <v>479</v>
       </c>
@@ -10921,7 +10924,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6">
       <c r="A481">
         <v>479</v>
       </c>
@@ -10935,7 +10938,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:6">
       <c r="A482">
         <v>479</v>
       </c>
@@ -10952,7 +10955,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:6">
       <c r="A483">
         <v>479</v>
       </c>
@@ -10969,7 +10972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:6">
       <c r="A484">
         <v>479</v>
       </c>
@@ -10986,7 +10989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:6">
       <c r="A485">
         <v>479</v>
       </c>
@@ -11003,7 +11006,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:6">
       <c r="A486">
         <v>479</v>
       </c>
@@ -11020,7 +11023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:6">
       <c r="A487">
         <v>479</v>
       </c>
@@ -11034,7 +11037,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:6">
       <c r="A488">
         <v>479</v>
       </c>
@@ -11048,7 +11051,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:6">
       <c r="A489">
         <v>479</v>
       </c>
@@ -11062,7 +11065,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:6">
       <c r="A490">
         <v>479</v>
       </c>
@@ -11076,7 +11079,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:6">
       <c r="A491">
         <v>479</v>
       </c>
@@ -11093,7 +11096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:6">
       <c r="A492">
         <v>479</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:6">
       <c r="A493">
         <v>479</v>
       </c>
@@ -11127,7 +11130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:6">
       <c r="A494">
         <v>479</v>
       </c>
@@ -11144,7 +11147,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:6">
       <c r="A495">
         <v>479</v>
       </c>
@@ -11158,7 +11161,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:6">
       <c r="A496">
         <v>479</v>
       </c>
@@ -11172,7 +11175,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6">
       <c r="A497">
         <v>479</v>
       </c>
@@ -11189,7 +11192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6">
       <c r="A498">
         <v>479</v>
       </c>
@@ -11203,7 +11206,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:6">
       <c r="A499">
         <v>479</v>
       </c>
@@ -11220,7 +11223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:6">
       <c r="A500">
         <v>479</v>
       </c>
@@ -11237,7 +11240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:6">
       <c r="A501">
         <v>479</v>
       </c>
@@ -11254,7 +11257,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:6">
       <c r="A502">
         <v>479</v>
       </c>
@@ -11271,7 +11274,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:6">
       <c r="A503">
         <v>479</v>
       </c>
@@ -11288,7 +11291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:6">
       <c r="A504">
         <v>479</v>
       </c>
@@ -11305,7 +11308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:6">
       <c r="A505">
         <v>479</v>
       </c>
@@ -11322,7 +11325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:6">
       <c r="A506">
         <v>479</v>
       </c>
@@ -11339,7 +11342,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:6">
       <c r="A507">
         <v>479</v>
       </c>
@@ -11356,7 +11359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:6">
       <c r="A508">
         <v>479</v>
       </c>
@@ -11373,7 +11376,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:6">
       <c r="A509">
         <v>479</v>
       </c>
@@ -11390,7 +11393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:6">
       <c r="A510">
         <v>479</v>
       </c>
@@ -11407,7 +11410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:6">
       <c r="A511">
         <v>479</v>
       </c>
@@ -11424,7 +11427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:6">
       <c r="A512">
         <v>479</v>
       </c>
@@ -11441,7 +11444,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:6">
       <c r="A513">
         <v>479</v>
       </c>
@@ -11458,7 +11461,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:6">
       <c r="A514">
         <v>479</v>
       </c>
@@ -11475,7 +11478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:6">
       <c r="A515">
         <v>479</v>
       </c>
@@ -11489,7 +11492,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:6">
       <c r="A516">
         <v>479</v>
       </c>
@@ -11506,7 +11509,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:6">
       <c r="A517">
         <v>479</v>
       </c>
@@ -11520,7 +11523,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:6">
       <c r="A518">
         <v>479</v>
       </c>
@@ -11534,7 +11537,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:6">
       <c r="A519">
         <v>479</v>
       </c>
@@ -11551,7 +11554,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:6">
       <c r="A520">
         <v>479</v>
       </c>
@@ -11568,7 +11571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:6">
       <c r="A521">
         <v>479</v>
       </c>
@@ -11585,7 +11588,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:6">
       <c r="A522">
         <v>479</v>
       </c>
@@ -11602,7 +11605,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:6">
       <c r="A523">
         <v>479</v>
       </c>
@@ -11616,7 +11619,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:6">
       <c r="A524">
         <v>479</v>
       </c>

</xml_diff>